<commit_message>
:art: :mag: Set of coherent tags <title> and <meta name=description> on the site and re order of indentations on head
</commit_message>
<xml_diff>
--- a/audit_ligthouse/0_audit_SEO.xlsx
+++ b/audit_ligthouse/0_audit_SEO.xlsx
@@ -88,10 +88,10 @@
     <t xml:space="preserve">https://webaim.org/standards/wcag/checklist#sc3.1.1   https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055281-creez-du-contenu-pour-chaque-langue </t>
   </si>
   <si>
-    <t xml:space="preserve">Les balises META &lt;title&gt; et &lt;description&gt; sont vides ou ont du contenu pas clair par rapport au contenu de la page chargée.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Idéalement, le &lt;title&gt; ne doit pas dépasser les 65 caractères et doit avoir un texte indicatif au contenu de la page. EN autre,  la  &lt;description&gt; doit avoir entre 70 et 320 caractères.</t>
+    <t xml:space="preserve">Les balises &lt;title&gt; et meta &lt;description&gt; sont vides ou ont du contenu pas clair par rapport au contenu de la page chargée.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Idéalement, le &lt;title&gt; ne doit pas dépasser les 65 caractères et doit avoir un texte indicatif au contenu de la page. En autre,  la  balise META &lt;description&gt; doit avoir entre 70 et 320 caractères.</t>
   </si>
   <si>
     <t xml:space="preserve">Rédiger correctement les balises associées au titre et à la description pour le site dans la section &lt;head&gt;.</t>
@@ -323,6 +323,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -485,20 +486,20 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="41.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="10.56"/>
   </cols>
   <sheetData>
@@ -1867,17 +1868,17 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist"/>
-    <hyperlink ref="F3" r:id="rId2" display="https://developer.mozilla.org/fr/docs/Glossary/Favicon"/>
-    <hyperlink ref="F7" r:id="rId3" display="https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578338-reconnaissez-les-differents-types-de-mots-cles"/>
-    <hyperlink ref="F8" r:id="rId4" display="https://developer.mozilla.org/en-US/docs/Learn/HTML/Howto/Author_fast-loading_HTML_pages"/>
-    <hyperlink ref="F9" r:id="rId5" display="https://developer.mozilla.org/en-US/docs/Web/HTML/Element"/>
+    <hyperlink ref="F3" r:id="rId2" display="https://developer.mozilla.org/fr/docs/Glossary/Favicon "/>
+    <hyperlink ref="F7" r:id="rId3" display="https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578338-reconnaissez-les-differents-types-de-mots-cles "/>
+    <hyperlink ref="F8" r:id="rId4" display="https://developer.mozilla.org/en-US/docs/Learn/HTML/Howto/Author_fast-loading_HTML_pages "/>
+    <hyperlink ref="F9" r:id="rId5" display="https://developer.mozilla.org/en-US/docs/Web/HTML/Element "/>
     <hyperlink ref="F10" r:id="rId6" display="https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links?hl=fr"/>
-    <hyperlink ref="F13" r:id="rId7" display="https://www.w3.org/WAI/WCAG21/Understanding/contrast-minimum.html"/>
-    <hyperlink ref="F14" r:id="rId8" display="https://www.w3.org/WAI/WCAG21/Understanding/link-purpose-in-context.html"/>
-    <hyperlink ref="F15" r:id="rId9" display="https://www.w3.org/WAI/WCAG21/Understanding/link-purpose-in-context.html"/>
-    <hyperlink ref="F16" r:id="rId10" location="sc2.4.4" display="https://webaim.org/standards/wcag/checklist#sc2.4.4"/>
-    <hyperlink ref="F17" r:id="rId11" display="https://web.dev/uses-optimized-images/?utm_source=lighthouse&amp;utm_medium=devtools"/>
-    <hyperlink ref="F18" r:id="rId12" display="https://developer.mozilla.org/en-US/docs/Learn/Forms/How_to_structure_a_web_form"/>
+    <hyperlink ref="F13" r:id="rId7" display=" https://www.w3.org/WAI/WCAG21/Understanding/contrast-minimum.html "/>
+    <hyperlink ref="F14" r:id="rId8" display="https://www.w3.org/WAI/WCAG21/Understanding/link-purpose-in-context.html "/>
+    <hyperlink ref="F15" r:id="rId9" display="https://www.w3.org/WAI/WCAG21/Understanding/link-purpose-in-context.html "/>
+    <hyperlink ref="F16" r:id="rId10" location="sc2.4.4" display="https://webaim.org/standards/wcag/checklist#sc2.4.4 "/>
+    <hyperlink ref="F17" r:id="rId11" display="https://web.dev/uses-optimized-images/?utm_source=lighthouse&amp;utm_medium=devtools "/>
+    <hyperlink ref="F18" r:id="rId12" display="https://developer.mozilla.org/en-US/docs/Learn/Forms/How_to_structure_a_web_form "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
:fire: :mag: removal of hiddent text that does not compile with acessibility neither SEO guidelines
</commit_message>
<xml_diff>
--- a/audit_ligthouse/0_audit_SEO.xlsx
+++ b/audit_ligthouse/0_audit_SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="83">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">Ajouter la langue de la page dans la balise html</t>
   </si>
   <si>
-    <t xml:space="preserve">https://webaim.org/standards/wcag/checklist#sc3.1.1   https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055281-creez-du-contenu-pour-chaque-langue </t>
+    <t xml:space="preserve">https://webaim.org/standards/wcag/checklist#sc3.1.1    https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055281-creez-du-contenu-pour-chaque-langue   </t>
   </si>
   <si>
     <t xml:space="preserve">Les balises &lt;title&gt; et meta &lt;description&gt; sont vides ou ont du contenu pas clair par rapport au contenu de la page chargée.</t>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">Rédiger correctement les balises associées au titre et à la description pour le site dans la section &lt;head&gt;.</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html  https://www.w3.org/TR/WCAG21/#page-titled </t>
+    <t xml:space="preserve">https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html   https://www.w3.org/TR/WCAG21/#page-titled  </t>
   </si>
   <si>
     <t xml:space="preserve">Le site n’a pas une tag pour être indexé.</t>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">Ajouter le tag d’indexation dans la section &lt;head&gt;.</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html   https://support.google.com/analytics/answer/1008080?hl=fr#zippy=%2Csite-web-statique </t>
+    <t xml:space="preserve">https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html    https://support.google.com/analytics/answer/1008080?hl=fr#zippy=%2Csite-web-statique  </t>
   </si>
   <si>
     <t xml:space="preserve">Les mots-clés utilisés ne sont pas optimaux.</t>
@@ -151,10 +151,10 @@
     <t xml:space="preserve">https://developer.mozilla.org/en-US/docs/Web/HTML/Element </t>
   </si>
   <si>
-    <t xml:space="preserve">Dans la section de navigation de la page principale,  il y a du texte à faible contraste sur un fond blanc (ratio 1.6:1). Pour la page du formulaire il y a du texte caché en dessous de la bannière .  Egalement, du texte caché est présent dans le footer de la page principale.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ces élément peuvent pénaliser  le SEO et ne sont pas des bonnes pratiques.</t>
+    <t xml:space="preserve">Dans la section de navigation de la page principale,  il y a du texte à faible contraste sur un fond blanc (ratio 1.6:1).  Et il existe du texte caché dans le footer de la page principale.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ces élément peuvent pénaliser le SEO et ne sont pas des bonnes pratiques.</t>
   </si>
   <si>
     <t xml:space="preserve">Enlever le texte pour ces parties. </t>
@@ -163,6 +163,18 @@
     <t xml:space="preserve">https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links?hl=fr</t>
   </si>
   <si>
+    <t xml:space="preserve">Pour la page du formulaire, il y a du texte caché dans la bannière/barre orange.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le contraste du texte a un ratio inférieur à 4.5:1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Il faut que le contenu soit lisible et dans les balises sémantiques adéquates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3.org/TR/WCAG21/#contrast-minimum </t>
+  </si>
+  <si>
     <t xml:space="preserve">Performance, Accessibilité</t>
   </si>
   <si>
@@ -175,7 +187,7 @@
     <t xml:space="preserve">Harmoniser les section header et footer dans le site en utilisant les balises sémantiques pertinentes.  Le menu déroulant dans la section de navigation peut être remplacé par un menu plus simple en HTML/CSS. </t>
   </si>
   <si>
-    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Learn/HTML/Introduction_to_HTML/Document_and_website_structure  https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055256-decouvrez-comment-google-interprete-le-javascript  https://webaim.org/standards/wcag/checklist#sc2.4.4 </t>
+    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Learn/HTML/Introduction_to_HTML/Document_and_website_structure   https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055256-decouvrez-comment-google-interprete-le-javascript   https://webaim.org/standards/wcag/checklist#sc2.4.4  </t>
   </si>
   <si>
     <t xml:space="preserve">Le texte dans le site (documents, buttons, descriptions) n’a pas le contraste ni la taille adéquats pour les utilisateur ayant une vision limitée.</t>
@@ -187,7 +199,7 @@
     <t xml:space="preserve">Modifier la couleur et la taille du texte pour compiler avec les standards.</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://www.w3.org/WAI/WCAG21/Understanding/contrast-minimum.html   https://www.w3.org/TR/WCAG21/#dfn-text </t>
+    <t xml:space="preserve"> https://www.w3.org/WAI/WCAG21/Understanding/contrast-minimum.html    https://www.w3.org/TR/WCAG21/#dfn-text  </t>
   </si>
   <si>
     <t xml:space="preserve">Dans la page principale, il y a des images contenant du texte.</t>
@@ -266,7 +278,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -317,6 +329,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="12"/>
@@ -374,7 +392,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -388,23 +406,31 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -486,20 +512,20 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="37.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="83.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="10.56"/>
   </cols>
   <sheetData>
@@ -559,7 +585,7 @@
       <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -579,7 +605,7 @@
       <c r="E3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -599,7 +625,7 @@
       <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -619,15 +645,15 @@
       <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="61.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -639,12 +665,12 @@
       <c r="E6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="62.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -659,12 +685,12 @@
       <c r="E7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="70.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -679,7 +705,7 @@
       <c r="E8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="6" t="s">
         <v>38</v>
       </c>
     </row>
@@ -699,12 +725,12 @@
       <c r="E9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="120.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+    <row r="10" customFormat="false" ht="101.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -713,39 +739,39 @@
       <c r="C10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="7" t="s">
         <v>45</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="105.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="60.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="100.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
-        <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>52</v>
@@ -759,12 +785,12 @@
       <c r="E12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="50.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
+    <row r="13" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -779,13 +805,13 @@
       <c r="E13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
-        <v>17</v>
+    <row r="14" customFormat="false" ht="50.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>60</v>
@@ -799,13 +825,13 @@
       <c r="E14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
-        <v>6</v>
+    <row r="15" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>64</v>
@@ -819,33 +845,33 @@
       <c r="E15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>63</v>
+      <c r="F15" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="45.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
+    <row r="16" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>70</v>
+      <c r="F16" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="78.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
-        <v>34</v>
+    <row r="17" customFormat="false" ht="45.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>71</v>
@@ -859,12 +885,12 @@
       <c r="E17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="42.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
+    <row r="18" customFormat="false" ht="78.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="4" t="s">
@@ -879,11 +905,30 @@
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="42.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1854,7 +1899,7 @@
     <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="988" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="989" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="990" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1873,12 +1918,13 @@
     <hyperlink ref="F8" r:id="rId4" display="https://developer.mozilla.org/en-US/docs/Learn/HTML/Howto/Author_fast-loading_HTML_pages "/>
     <hyperlink ref="F9" r:id="rId5" display="https://developer.mozilla.org/en-US/docs/Web/HTML/Element "/>
     <hyperlink ref="F10" r:id="rId6" display="https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links?hl=fr"/>
-    <hyperlink ref="F13" r:id="rId7" display=" https://www.w3.org/WAI/WCAG21/Understanding/contrast-minimum.html "/>
-    <hyperlink ref="F14" r:id="rId8" display="https://www.w3.org/WAI/WCAG21/Understanding/link-purpose-in-context.html "/>
+    <hyperlink ref="F11" r:id="rId7" location="contrast-minimum" display="https://www.w3.org/TR/WCAG21/#contrast-minimum"/>
+    <hyperlink ref="F14" r:id="rId8" display=" https://www.w3.org/WAI/WCAG21/Understanding/contrast-minimum.html "/>
     <hyperlink ref="F15" r:id="rId9" display="https://www.w3.org/WAI/WCAG21/Understanding/link-purpose-in-context.html "/>
-    <hyperlink ref="F16" r:id="rId10" location="sc2.4.4" display="https://webaim.org/standards/wcag/checklist#sc2.4.4 "/>
-    <hyperlink ref="F17" r:id="rId11" display="https://web.dev/uses-optimized-images/?utm_source=lighthouse&amp;utm_medium=devtools "/>
-    <hyperlink ref="F18" r:id="rId12" display="https://developer.mozilla.org/en-US/docs/Learn/Forms/How_to_structure_a_web_form "/>
+    <hyperlink ref="F16" r:id="rId10" display="https://www.w3.org/WAI/WCAG21/Understanding/link-purpose-in-context.html "/>
+    <hyperlink ref="F17" r:id="rId11" location="sc2.4.4" display="https://webaim.org/standards/wcag/checklist#sc2.4.4 "/>
+    <hyperlink ref="F18" r:id="rId12" display="https://web.dev/uses-optimized-images/?utm_source=lighthouse&amp;utm_medium=devtools "/>
+    <hyperlink ref="F19" r:id="rId13" display="https://developer.mozilla.org/en-US/docs/Learn/Forms/How_to_structure_a_web_form "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
:art: :fire: removal of unnecessary JS files and call of minified JS versions
</commit_message>
<xml_diff>
--- a/audit_ligthouse/0_audit_SEO.xlsx
+++ b/audit_ligthouse/0_audit_SEO.xlsx
@@ -133,16 +133,16 @@
     <t xml:space="preserve">Le site prends du temps supplémentaire à charger à cause des éléments inutilisés et le chargement de plusieurs fichiers.</t>
   </si>
   <si>
-    <t xml:space="preserve">Supprimer les fichiers JS et CSS non utilisés. Les autres fichiers doivent être « minifiées » et combinés pour réduire le temps du chargement. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://developer.mozilla.org/en-US/docs/Learn/HTML/Howto/Author_fast-loading_HTML_pages </t>
+    <t xml:space="preserve">Dans une première instance, supprimer les fichiers JS et CSS non utilisés. Ensuite, utiliser une version « minifiée »  pour augmenter la performance. Et finalement, si possible combiner les fichiers similaires pour réduire le temps du chargement. Pour les fichiers JS utiliser l’attribut « defer ».</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://developer.mozilla.org/en-US/docs/Learn/HTML/Howto/Author_fast-loading_HTML_pages   https://discourse.mozilla.org/t/async-v-s-defer/53819/2   https://hacks.mozilla.org/2017/09/building-the-dom-faster-speculative-parsing-async-defer-and-preload/ </t>
   </si>
   <si>
     <t xml:space="preserve">Le site n’a pas des balises sémantiques.</t>
   </si>
   <si>
-    <t xml:space="preserve">Il y a un utilisation excessive des balises div dans le site.</t>
+    <t xml:space="preserve">Il y a une utilisation excessive des balises div dans le site.</t>
   </si>
   <si>
     <t xml:space="preserve">Utiliser des balises sémantiques dans la structure HTML &lt;body&gt; pour améliorer identifier l’objet du contenu dans les balises.</t>
@@ -262,13 +262,13 @@
     <t xml:space="preserve">La structure du formulaire de contact n’est pas correcte.</t>
   </si>
   <si>
-    <t xml:space="preserve">Absence des arguments obligatoires dans les  &lt;label&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ajouter les ID des différents inputs du formulaire.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://developer.mozilla.org/en-US/docs/Learn/Forms/How_to_structure_a_web_form </t>
+    <t xml:space="preserve">Absence des arguments obligatoires dans les balises &lt;label&gt; et besoin des éléments d’accessibilité.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajouter les identifiants (ID) des différents entrées du formulaire. Ajouter le rôle pour améliorer l’accessibilité.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://developer.mozilla.org/en-US/docs/Learn/Forms/How_to_structure_a_web_form  https://developer.mozilla.org/en-US/docs/Web/Accessibility/ARIA/Roles/Form_Role </t>
   </si>
 </sst>
 </file>
@@ -278,7 +278,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -329,12 +329,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="12"/>
@@ -392,7 +386,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -426,10 +420,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -512,13 +502,13 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.98"/>
@@ -689,7 +679,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="70.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="108" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
         <v>34</v>
       </c>
@@ -753,7 +743,7 @@
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -790,7 +780,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1915,16 +1905,14 @@
     <hyperlink ref="F2" r:id="rId1" display="https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist"/>
     <hyperlink ref="F3" r:id="rId2" display="https://developer.mozilla.org/fr/docs/Glossary/Favicon "/>
     <hyperlink ref="F7" r:id="rId3" display="https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578338-reconnaissez-les-differents-types-de-mots-cles "/>
-    <hyperlink ref="F8" r:id="rId4" display="https://developer.mozilla.org/en-US/docs/Learn/HTML/Howto/Author_fast-loading_HTML_pages "/>
-    <hyperlink ref="F9" r:id="rId5" display="https://developer.mozilla.org/en-US/docs/Web/HTML/Element "/>
-    <hyperlink ref="F10" r:id="rId6" display="https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links?hl=fr"/>
-    <hyperlink ref="F11" r:id="rId7" location="contrast-minimum" display="https://www.w3.org/TR/WCAG21/#contrast-minimum"/>
-    <hyperlink ref="F14" r:id="rId8" display=" https://www.w3.org/WAI/WCAG21/Understanding/contrast-minimum.html "/>
-    <hyperlink ref="F15" r:id="rId9" display="https://www.w3.org/WAI/WCAG21/Understanding/link-purpose-in-context.html "/>
-    <hyperlink ref="F16" r:id="rId10" display="https://www.w3.org/WAI/WCAG21/Understanding/link-purpose-in-context.html "/>
-    <hyperlink ref="F17" r:id="rId11" location="sc2.4.4" display="https://webaim.org/standards/wcag/checklist#sc2.4.4 "/>
-    <hyperlink ref="F18" r:id="rId12" display="https://web.dev/uses-optimized-images/?utm_source=lighthouse&amp;utm_medium=devtools "/>
-    <hyperlink ref="F19" r:id="rId13" display="https://developer.mozilla.org/en-US/docs/Learn/Forms/How_to_structure_a_web_form "/>
+    <hyperlink ref="F9" r:id="rId4" display="https://developer.mozilla.org/en-US/docs/Web/HTML/Element "/>
+    <hyperlink ref="F10" r:id="rId5" display="https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links?hl=fr"/>
+    <hyperlink ref="F11" r:id="rId6" location="contrast-minimum" display="https://www.w3.org/TR/WCAG21/#contrast-minimum "/>
+    <hyperlink ref="F14" r:id="rId7" display=" https://www.w3.org/WAI/WCAG21/Understanding/contrast-minimum.html "/>
+    <hyperlink ref="F15" r:id="rId8" display="https://www.w3.org/WAI/WCAG21/Understanding/link-purpose-in-context.html "/>
+    <hyperlink ref="F16" r:id="rId9" display="https://www.w3.org/WAI/WCAG21/Understanding/link-purpose-in-context.html "/>
+    <hyperlink ref="F17" r:id="rId10" location="sc2.4.4" display="https://webaim.org/standards/wcag/checklist#sc2.4.4 "/>
+    <hyperlink ref="F18" r:id="rId11" display="https://web.dev/uses-optimized-images/?utm_source=lighthouse&amp;utm_medium=devtools "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
:mag: addition of the meta tag for indexation on search engines
</commit_message>
<xml_diff>
--- a/audit_ligthouse/0_audit_SEO.xlsx
+++ b/audit_ligthouse/0_audit_SEO.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Les titres ne respectent pas un ordre hiérarchique.</t>
   </si>
   <si>
-    <t xml:space="preserve">Les balises h3 présentes dans la page index ne sont pas dans l’intérieur d’une balise h2.</t>
+    <t xml:space="preserve">Les balises h3 présentes dans la page index ne sont pas à l’intérieur d’une balise h2.</t>
   </si>
   <si>
     <t xml:space="preserve">Organiser correctement le code HTML.</t>
@@ -58,6 +58,132 @@
     <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist</t>
   </si>
   <si>
+    <t xml:space="preserve">Le site n’a pas des balises sémantiques.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il y a une utilisation excessive des balises div dans le site.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utiliser des balises sémantiques dans la structure HTML &lt;body&gt; pour améliorer l’identification du contenu dans les balises.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://developer.mozilla.org/en-US/docs/Web/HTML/Element </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pour la page du formulaire, il y a du texte caché dans la bannière/barre orange.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le contraste du texte a un ratio inférieur à 4.5:1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Il faut que le contenu soit lisible et dans les balises sémantiques adéquates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3.org/TR/WCAG21/#contrast-minimum </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dans la page principale, il y a des images contenant du texte.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les images contenant du texte doivent être évitées</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Effacer les images contenant du texte et ajouter leur contenu sous forme du texte en HTML</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://www.w3.org/WAI/WCAG21/Understanding/contrast-minimum.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le nom de la page de contact a été défini comme  « page 2 ». </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le nom des liens ne doit pas être ambigu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changer le nom du fichier « page2.html » par « contact.html »</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.w3.org/WAI/WCAG21/Understanding/link-purpose-in-context.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les icônes associés aux réseaux sociaux ont des liens vides.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dans l’absence du lien, aucune information sera présenté à l’utilisateur.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajouter les liens correspondant aux réseaux sociaux.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://webaim.org/standards/wcag/checklist#sc2.4.4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le texte dans le site (documents, buttons, descriptions) n’a pas le contraste ni la taille adéquats pour les utilisateur ayant une vision limitée.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le contraste minimal requis est d’un ratio 4.5:1 et la police doit avoir au minimum 14pt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modifier la couleur et la taille du texte pour compiler avec les standards.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://www.w3.org/WAI/WCAG21/Understanding/contrast-minimum.html    https://www.w3.org/TR/WCAG21/#dfn-text  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accessibilité, Performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le header et le footer ne sont pas homogènes dans le site.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’affichage du header et du footer est différent dans les différentes pages.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harmoniser les section header et footer dans le site en utilisant les balises sémantiques pertinentes.  Le menu déroulant dans la section de navigation peut être remplacé par un menu plus simple en HTML/CSS. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Learn/HTML/Introduction_to_HTML/Document_and_website_structure   https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055256-decouvrez-comment-google-interprete-le-javascript   https://webaim.org/standards/wcag/checklist#sc2.4.4  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La page principale prend plus de 17s seconds à charger.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les images utilisées ne sont pas optimisées. Le format bmp n’est pas adéquat .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compresser les images et utiliser un format et taille adéquats pour un chargement plus rapide.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.dev/uses-optimized-images/?utm_source=lighthouse&amp;utm_medium=devtools </t>
+  </si>
+  <si>
+    <t xml:space="preserve">La structure du formulaire de contact n’est pas correcte.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absence des arguments obligatoires dans les balises &lt;label&gt; et besoin des éléments d’accessibilité.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajouter les identifiants (ID) des différents entrées du formulaire. Ajouter le rôle pour améliorer l’accessibilité.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://developer.mozilla.org/en-US/docs/Learn/Forms/How_to_structure_a_web_form  https://developer.mozilla.org/en-US/docs/Web/Accessibility/ARIA/Roles/Form_Role </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il existent des éléments JS et CSS qui ne sont pas utilisés dans le site web. Et il y a plusieurs fichiers CSS et JS au chargement du site.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le site prends du temps supplémentaire à charger à cause des éléments inutilisés et le chargement de plusieurs fichiers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dans une première instance, supprimer les fichiers JS et CSS non utilisés. Ensuite, utiliser une version « minifiée »  pour augmenter la performance. Et finalement, si possible combiner les fichiers similaires pour réduire le temps du chargement. Pour les fichiers JS utiliser l’attribut « defer ».</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://developer.mozilla.org/en-US/docs/Learn/HTML/Howto/Author_fast-loading_HTML_pages   https://discourse.mozilla.org/t/async-v-s-defer/53819/2   https://hacks.mozilla.org/2017/09/building-the-dom-faster-speculative-parsing-async-defer-and-preload/ </t>
+  </si>
+  <si>
     <t xml:space="preserve">Structure</t>
   </si>
   <si>
@@ -109,7 +235,7 @@
     <t xml:space="preserve">Ajouter le tag d’indexation dans la section &lt;head&gt;.</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html    https://support.google.com/analytics/answer/1008080?hl=fr#zippy=%2Csite-web-statique  </t>
+    <t xml:space="preserve">https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html    https://support.google.com/analytics/answer/1008080?hl=fr#zippy=%2Csite-web-statique  https://support.google.com/webmasters/answer/9008080#meta_tag_verification</t>
   </si>
   <si>
     <t xml:space="preserve">Les mots-clés utilisés ne sont pas optimaux.</t>
@@ -118,39 +244,30 @@
     <t xml:space="preserve">Les mots-clés (ou keywords) sont très similaires et ont un trafic bas et concurrence élevée.</t>
   </si>
   <si>
-    <t xml:space="preserve">Optimiser les mots-clés avec un bon compromis entre haut trafic et  concurrence faible/moyenne.</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Optimiser les mots-clés avec un bon compromis entre haut trafic et  concurrence faible/moyenne. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Liberation Sans Serif"/>
+        <family val="2"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve">Une étude des mots-clés est fortement recommandée. </t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578338-reconnaissez-les-differents-types-de-mots-cles </t>
   </si>
   <si>
-    <t xml:space="preserve">Performance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Il existent des éléments JS et CSS qui ne sont pas utilisés dans le site web. Et il y a plusieurs fichiers CSS et JS au chargement du site.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le site prends du temps supplémentaire à charger à cause des éléments inutilisés et le chargement de plusieurs fichiers.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dans une première instance, supprimer les fichiers JS et CSS non utilisés. Ensuite, utiliser une version « minifiée »  pour augmenter la performance. Et finalement, si possible combiner les fichiers similaires pour réduire le temps du chargement. Pour les fichiers JS utiliser l’attribut « defer ».</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://developer.mozilla.org/en-US/docs/Learn/HTML/Howto/Author_fast-loading_HTML_pages   https://discourse.mozilla.org/t/async-v-s-defer/53819/2   https://hacks.mozilla.org/2017/09/building-the-dom-faster-speculative-parsing-async-defer-and-preload/ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le site n’a pas des balises sémantiques.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Il y a une utilisation excessive des balises div dans le site.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Utiliser des balises sémantiques dans la structure HTML &lt;body&gt; pour améliorer identifier l’objet du contenu dans les balises.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://developer.mozilla.org/en-US/docs/Web/HTML/Element </t>
-  </si>
-  <si>
     <t xml:space="preserve">Dans la section de navigation de la page principale,  il y a du texte à faible contraste sur un fond blanc (ratio 1.6:1).  Et il existe du texte caché dans le footer de la page principale.</t>
   </si>
   <si>
@@ -163,57 +280,6 @@
     <t xml:space="preserve">https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links?hl=fr</t>
   </si>
   <si>
-    <t xml:space="preserve">Pour la page du formulaire, il y a du texte caché dans la bannière/barre orange.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le contraste du texte a un ratio inférieur à 4.5:1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Il faut que le contenu soit lisible et dans les balises sémantiques adéquates</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.w3.org/TR/WCAG21/#contrast-minimum </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Performance, Accessibilité</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le header et le footer ne sont pas homogènes dans le site.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L’affichage du header et du footer est différent dans les différentes pages.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Harmoniser les section header et footer dans le site en utilisant les balises sémantiques pertinentes.  Le menu déroulant dans la section de navigation peut être remplacé par un menu plus simple en HTML/CSS. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://developer.mozilla.org/fr/docs/Learn/HTML/Introduction_to_HTML/Document_and_website_structure   https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055256-decouvrez-comment-google-interprete-le-javascript   https://webaim.org/standards/wcag/checklist#sc2.4.4  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le texte dans le site (documents, buttons, descriptions) n’a pas le contraste ni la taille adéquats pour les utilisateur ayant une vision limitée.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le contraste minimal requis est du ratio 4.5:1 et la police doit avoir au minimum 14pt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modifier la couleur et la taille du texte pour compiler avec les standards.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> https://www.w3.org/WAI/WCAG21/Understanding/contrast-minimum.html    https://www.w3.org/TR/WCAG21/#dfn-text  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dans la page principale, il y a des images contenant du texte.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les images contenant du texte doivent être évitées</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Changer les images contenant du texte pour du contenu du texte en HTML</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> https://www.w3.org/WAI/WCAG21/Understanding/contrast-minimum.html </t>
-  </si>
-  <si>
     <t xml:space="preserve">Dans le footer, les sections d’annuaires doivent disparaître.</t>
   </si>
   <si>
@@ -221,54 +287,6 @@
   </si>
   <si>
     <t xml:space="preserve">Vérifier la cohérence du contenu des liens. Eventuellement, supprimer cette section.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.w3.org/WAI/WCAG21/Understanding/link-purpose-in-context.html </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le nom de la page de contact a été défini comme  « page 2 ». </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le nom des liens ne doit pas être ambigu.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Changer le nom du fichier « page2.html » ver « contact.html »</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les icônes associés aux réseaux sociaux ont des liens vides.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dans l’absence du lien, aucune information sera présenté à l’utilisateur.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ajouter les liens correspondant aux réseaux sociaux.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://webaim.org/standards/wcag/checklist#sc2.4.4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">La page principale prend plus de 17s seconds à charger.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les images utilisées ne sont pas optimisées. Le format bmp n’est pas adéquat .</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compresser les images et utiliser un format et taille adéquats pour un chargement plus rapide sur la version desktop du site.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://web.dev/uses-optimized-images/?utm_source=lighthouse&amp;utm_medium=devtools </t>
-  </si>
-  <si>
-    <t xml:space="preserve">La structure du formulaire de contact n’est pas correcte.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Absence des arguments obligatoires dans les balises &lt;label&gt; et besoin des éléments d’accessibilité.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ajouter les identifiants (ID) des différents entrées du formulaire. Ajouter le rôle pour améliorer l’accessibilité.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://developer.mozilla.org/en-US/docs/Learn/Forms/How_to_structure_a_web_form  https://developer.mozilla.org/en-US/docs/Web/Accessibility/ARIA/Roles/Form_Role </t>
   </si>
 </sst>
 </file>
@@ -305,8 +323,8 @@
       <b val="true"/>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Cambria"/>
-      <family val="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
@@ -319,23 +337,22 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Liberation Sans Serif"/>
+      <family val="2"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="3">
@@ -386,7 +403,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -403,7 +420,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -411,15 +428,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -502,20 +515,20 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.46875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="37.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="83.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="41.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="58.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="10.56"/>
   </cols>
   <sheetData>
@@ -579,229 +592,229 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="65.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="53.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="53.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="47.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="53.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="74.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="53.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="61.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="D6" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>28</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="53.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="62.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F7" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="53.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="108" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
+      <c r="D8" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="104.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="66.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="86.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="101.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>45</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="75.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="60.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="111.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="100.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F12" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="65.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>57</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="47.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="50.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
-        <v>6</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>60</v>
@@ -819,9 +832,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
-        <v>17</v>
+    <row r="15" customFormat="false" ht="74.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>64</v>
@@ -839,11 +852,11 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="61.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -856,67 +869,67 @@
         <v>10</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="45.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="62.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="78.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
-        <v>34</v>
+    <row r="18" customFormat="false" ht="101.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="4" t="s">
         <v>77</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="42.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="63.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>10</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1888,8 +1901,8 @@
     <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="988" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="989" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="990" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1903,16 +1916,17 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" display="https://developer.mozilla.org/fr/docs/Web/Accessibility/Mobile_accessibility_checklist"/>
-    <hyperlink ref="F3" r:id="rId2" display="https://developer.mozilla.org/fr/docs/Glossary/Favicon "/>
-    <hyperlink ref="F7" r:id="rId3" display="https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578338-reconnaissez-les-differents-types-de-mots-cles "/>
-    <hyperlink ref="F9" r:id="rId4" display="https://developer.mozilla.org/en-US/docs/Web/HTML/Element "/>
-    <hyperlink ref="F10" r:id="rId5" display="https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links?hl=fr"/>
-    <hyperlink ref="F11" r:id="rId6" location="contrast-minimum" display="https://www.w3.org/TR/WCAG21/#contrast-minimum "/>
-    <hyperlink ref="F14" r:id="rId7" display=" https://www.w3.org/WAI/WCAG21/Understanding/contrast-minimum.html "/>
-    <hyperlink ref="F15" r:id="rId8" display="https://www.w3.org/WAI/WCAG21/Understanding/link-purpose-in-context.html "/>
-    <hyperlink ref="F16" r:id="rId9" display="https://www.w3.org/WAI/WCAG21/Understanding/link-purpose-in-context.html "/>
-    <hyperlink ref="F17" r:id="rId10" location="sc2.4.4" display="https://webaim.org/standards/wcag/checklist#sc2.4.4 "/>
-    <hyperlink ref="F18" r:id="rId11" display="https://web.dev/uses-optimized-images/?utm_source=lighthouse&amp;utm_medium=devtools "/>
+    <hyperlink ref="F3" r:id="rId2" display="https://developer.mozilla.org/en-US/docs/Web/HTML/Element "/>
+    <hyperlink ref="F4" r:id="rId3" location="contrast-minimum" display="https://www.w3.org/TR/WCAG21/#contrast-minimum "/>
+    <hyperlink ref="F5" r:id="rId4" display=" https://www.w3.org/WAI/WCAG21/Understanding/contrast-minimum.html "/>
+    <hyperlink ref="F6" r:id="rId5" display="https://www.w3.org/WAI/WCAG21/Understanding/link-purpose-in-context.html "/>
+    <hyperlink ref="F7" r:id="rId6" location="sc2.4.4" display="https://webaim.org/standards/wcag/checklist#sc2.4.4 "/>
+    <hyperlink ref="F10" r:id="rId7" display="https://web.dev/uses-optimized-images/?utm_source=lighthouse&amp;utm_medium=devtools "/>
+    <hyperlink ref="F13" r:id="rId8" display="https://developer.mozilla.org/fr/docs/Glossary/Favicon "/>
+    <hyperlink ref="F16" r:id="rId9" location="meta_tag_verification" display="https://support.google.com/webmasters/answer/9008080#meta_tag_verification"/>
+    <hyperlink ref="F17" r:id="rId10" display="https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578338-reconnaissez-les-differents-types-de-mots-cles "/>
+    <hyperlink ref="F18" r:id="rId11" display="https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links?hl=fr"/>
+    <hyperlink ref="F19" r:id="rId12" display="https://www.w3.org/WAI/WCAG21/Understanding/link-purpose-in-context.html "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
:wheelchair: fixtures on accessibility tags to generate focusable icons
</commit_message>
<xml_diff>
--- a/audit_ligthouse/0_audit_SEO.xlsx
+++ b/audit_ligthouse/0_audit_SEO.xlsx
@@ -115,7 +115,7 @@
     <t xml:space="preserve">Ajouter les liens correspondant aux réseaux sociaux.</t>
   </si>
   <si>
-    <t xml:space="preserve">https://webaim.org/standards/wcag/checklist#sc2.4.4 </t>
+    <t xml:space="preserve">https://webaim.org/standards/wcag/checklist#sc2.4.4  https://fontawesome.com/how-to-use/on-the-web/other-topics/accessibility </t>
   </si>
   <si>
     <t xml:space="preserve">Le texte dans le site (documents, buttons, descriptions) n’a pas le contraste ni la taille adéquats pour les utilisateur ayant une vision limitée.</t>
@@ -516,12 +516,12 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.46875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.28"/>
@@ -1920,13 +1920,12 @@
     <hyperlink ref="F4" r:id="rId3" location="contrast-minimum" display="https://www.w3.org/TR/WCAG21/#contrast-minimum "/>
     <hyperlink ref="F5" r:id="rId4" display=" https://www.w3.org/WAI/WCAG21/Understanding/contrast-minimum.html "/>
     <hyperlink ref="F6" r:id="rId5" display="https://www.w3.org/WAI/WCAG21/Understanding/link-purpose-in-context.html "/>
-    <hyperlink ref="F7" r:id="rId6" location="sc2.4.4" display="https://webaim.org/standards/wcag/checklist#sc2.4.4 "/>
-    <hyperlink ref="F10" r:id="rId7" display="https://web.dev/uses-optimized-images/?utm_source=lighthouse&amp;utm_medium=devtools "/>
-    <hyperlink ref="F13" r:id="rId8" display="https://developer.mozilla.org/fr/docs/Glossary/Favicon "/>
-    <hyperlink ref="F16" r:id="rId9" location="meta_tag_verification" display="https://support.google.com/webmasters/answer/9008080#meta_tag_verification"/>
-    <hyperlink ref="F17" r:id="rId10" display="https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578338-reconnaissez-les-differents-types-de-mots-cles "/>
-    <hyperlink ref="F18" r:id="rId11" display="https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links?hl=fr"/>
-    <hyperlink ref="F19" r:id="rId12" display="https://www.w3.org/WAI/WCAG21/Understanding/link-purpose-in-context.html "/>
+    <hyperlink ref="F10" r:id="rId6" display="https://web.dev/uses-optimized-images/?utm_source=lighthouse&amp;utm_medium=devtools "/>
+    <hyperlink ref="F13" r:id="rId7" display="https://developer.mozilla.org/fr/docs/Glossary/Favicon "/>
+    <hyperlink ref="F16" r:id="rId8" location="meta_tag_verification" display="https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html    https://support.google.com/analytics/answer/1008080?hl=fr#zippy=%2Csite-web-statique  https://support.google.com/webmasters/answer/9008080#meta_tag_verification"/>
+    <hyperlink ref="F17" r:id="rId9" display="https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578338-reconnaissez-les-differents-types-de-mots-cles "/>
+    <hyperlink ref="F18" r:id="rId10" display="https://developers.google.com/search/docs/advanced/guidelines/hidden-text-links?hl=fr"/>
+    <hyperlink ref="F19" r:id="rId11" display="https://www.w3.org/WAI/WCAG21/Understanding/link-purpose-in-context.html "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>